<commit_message>
barcode added to templates
</commit_message>
<xml_diff>
--- a/application/views/rpt/ru/doc/schet-oplata.xlsx
+++ b/application/views/rpt/ru/doc/schet-oplata.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="2" r:id="rId1"/>
+    <sheet name="Счёт на оплату" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>{$v-&gt;a-&gt;company_name}</t>
   </si>
@@ -177,6 +177,12 @@
   </si>
   <si>
     <t>{$v-&gt;p-&gt;company_tax_id}  / {$v-&gt;p-&gt;company_tax_id2}</t>
+  </si>
+  <si>
+    <t>Штрихкод</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;product_barcode}</t>
   </si>
 </sst>
 </file>
@@ -262,7 +268,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -356,10 +362,46 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -371,10 +413,10 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -386,10 +428,10 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -401,70 +443,10 @@
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -473,56 +455,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -533,51 +469,103 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -587,35 +575,26 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -918,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" activeCellId="1" sqref="B4:I5 F7:I7"/>
+      <selection activeCell="S1" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -929,15 +908,17 @@
     <col min="1" max="1" width="1.109375" customWidth="1"/>
     <col min="2" max="3" width="2" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="6" max="6" width="6.77734375" customWidth="1"/>
     <col min="8" max="8" width="12.44140625" customWidth="1"/>
     <col min="9" max="9" width="3.88671875" customWidth="1"/>
     <col min="10" max="10" width="2.33203125" customWidth="1"/>
     <col min="11" max="13" width="3.44140625" customWidth="1"/>
     <col min="14" max="16" width="4.109375" customWidth="1"/>
     <col min="17" max="18" width="7.6640625" customWidth="1"/>
+    <col min="19" max="19" width="6.21875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:19" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
@@ -958,553 +939,562 @@
       <c r="Q1" s="13"/>
       <c r="R1" s="13"/>
     </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="2:19" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="49" t="s">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="10" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="9" t="s">
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="8" t="s">
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="48" t="s">
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="N5" s="48"/>
-      <c r="O5" s="48"/>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="48"/>
-      <c r="R5" s="48"/>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B6" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="48"/>
-      <c r="O6" s="48"/>
-      <c r="P6" s="48"/>
-      <c r="Q6" s="48"/>
-      <c r="R6" s="48"/>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="50" t="s">
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="8" t="s">
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="7" t="s">
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
-      <c r="O10" s="47"/>
-      <c r="P10" s="47"/>
-      <c r="Q10" s="47"/>
-      <c r="R10" s="47"/>
-    </row>
-    <row r="11" spans="2:18" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+    </row>
+    <row r="11" spans="2:19" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="B11" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="27"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="27"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="23" t="s">
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="23"/>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="29"/>
+      <c r="R13" s="29"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B14" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="23" t="s">
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="23"/>
-    </row>
-    <row r="15" spans="2:18" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="25" t="s">
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="29"/>
+      <c r="R14" s="29"/>
+    </row>
+    <row r="15" spans="2:19" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L15" s="44"/>
+      <c r="M15" s="44"/>
+      <c r="N15" s="44"/>
+      <c r="O15" s="44"/>
+      <c r="P15" s="44"/>
+      <c r="Q15" s="44"/>
+      <c r="R15" s="44"/>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B16" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="26" t="s">
+      <c r="C16" s="31"/>
+      <c r="D16" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="16" t="s">
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="26" t="s">
+      <c r="I16" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26" t="s">
+      <c r="J16" s="31"/>
+      <c r="K16" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26" t="s">
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26"/>
-      <c r="Q16" s="27" t="s">
+      <c r="O16" s="31"/>
+      <c r="P16" s="31"/>
+      <c r="Q16" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="R16" s="27"/>
-    </row>
-    <row r="17" spans="1:18" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="28" t="s">
+      <c r="R16" s="31"/>
+      <c r="S16" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29" t="s">
+      <c r="C17" s="33"/>
+      <c r="D17" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="17" t="s">
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="29" t="s">
+      <c r="I17" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29" t="s">
+      <c r="J17" s="33"/>
+      <c r="K17" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29" t="s">
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="O17" s="29"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="30" t="s">
+      <c r="O17" s="33"/>
+      <c r="P17" s="33"/>
+      <c r="Q17" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="R17" s="30"/>
-    </row>
-    <row r="18" spans="1:18" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="31" t="s">
+      <c r="R17" s="33"/>
+      <c r="S17" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="32" t="s">
+      <c r="C18" s="45"/>
+      <c r="D18" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="18" t="s">
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="I18" s="31" t="s">
+      <c r="I18" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="J18" s="31"/>
-      <c r="K18" s="33" t="s">
+      <c r="J18" s="45"/>
+      <c r="K18" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33"/>
-      <c r="N18" s="34" t="s">
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="O18" s="34"/>
-      <c r="P18" s="34"/>
-      <c r="Q18" s="35" t="s">
+      <c r="O18" s="49"/>
+      <c r="P18" s="49"/>
+      <c r="Q18" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="R18" s="35"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="H19" s="1" t="s">
+      <c r="R18" s="49"/>
+      <c r="S18" s="47" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H19" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="Q19" s="1" t="s">
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="Q19" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="R19" s="1"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="H20" s="1" t="s">
+      <c r="R19" s="28"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H20" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="Q20" s="1" t="s">
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
+      <c r="Q20" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="R20" s="1"/>
-    </row>
-    <row r="21" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="H21" s="36" t="s">
+      <c r="R20" s="28"/>
+    </row>
+    <row r="21" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H21" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="36"/>
-      <c r="O21" s="37" t="s">
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="P21" s="37"/>
-      <c r="Q21" s="37"/>
-      <c r="R21" s="37"/>
-    </row>
-    <row r="22" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="20"/>
-    </row>
-    <row r="23" spans="1:18" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="B23" s="38" t="s">
+      <c r="P21" s="35"/>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="35"/>
+    </row>
+    <row r="22" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+    </row>
+    <row r="23" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="B23" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="38"/>
-      <c r="K23" s="38"/>
-      <c r="L23" s="38"/>
-      <c r="M23" s="38"/>
-      <c r="N23" s="38"/>
-      <c r="O23" s="38"/>
-      <c r="P23" s="38"/>
-      <c r="Q23" s="38"/>
-      <c r="R23" s="38"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B24" s="39" t="s">
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="40"/>
+      <c r="O23" s="40"/>
+      <c r="P23" s="40"/>
+      <c r="Q23" s="40"/>
+      <c r="R23" s="40"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B24" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="39"/>
-      <c r="N24" s="39"/>
-      <c r="O24" s="39"/>
-      <c r="P24" s="39"/>
-      <c r="Q24" s="39"/>
-      <c r="R24" s="39"/>
-    </row>
-    <row r="26" spans="1:18" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="44" t="s">
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="41"/>
+      <c r="K24" s="41"/>
+      <c r="L24" s="41"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
+      <c r="O24" s="41"/>
+      <c r="P24" s="41"/>
+      <c r="Q24" s="41"/>
+      <c r="R24" s="41"/>
+    </row>
+    <row r="26" spans="1:19" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="40"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="41" t="s">
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="M26" s="41"/>
-      <c r="N26" s="41"/>
-      <c r="O26" s="41"/>
-      <c r="P26" s="41"/>
-      <c r="Q26" s="41"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="42" t="s">
+      <c r="M26" s="39"/>
+      <c r="N26" s="39"/>
+      <c r="O26" s="39"/>
+      <c r="P26" s="39"/>
+      <c r="Q26" s="39"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="45" t="s">
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="M27" s="45"/>
-      <c r="N27" s="45"/>
-      <c r="O27" s="45"/>
-      <c r="P27" s="45"/>
-      <c r="Q27" s="45"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I28" s="22" t="s">
+      <c r="M27" s="38"/>
+      <c r="N27" s="38"/>
+      <c r="O27" s="38"/>
+      <c r="P27" s="38"/>
+      <c r="Q27" s="38"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I28" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="43" t="s">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="43"/>
-      <c r="L29" s="43"/>
-      <c r="M29" s="43"/>
-      <c r="N29" s="43"/>
-      <c r="O29" s="43"/>
-      <c r="P29" s="43"/>
-      <c r="Q29" s="43"/>
-      <c r="R29" s="43"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="36"/>
+      <c r="N29" s="36"/>
+      <c r="O29" s="36"/>
+      <c r="P29" s="36"/>
+      <c r="Q29" s="36"/>
+      <c r="R29" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="55">
@@ -1522,11 +1512,6 @@
     <mergeCell ref="Q20:R20"/>
     <mergeCell ref="H21:N21"/>
     <mergeCell ref="O21:R21"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="N18:P18"/>
     <mergeCell ref="Q18:R18"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="D17:G17"/>
@@ -1534,6 +1519,11 @@
     <mergeCell ref="K17:M17"/>
     <mergeCell ref="N17:P17"/>
     <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="N18:P18"/>
     <mergeCell ref="L15:R15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:G16"/>

</xml_diff>